<commit_message>
Reageret på feedback med flere kodekommentar mm
Fået Excel til at gemme rigtigt, og har fået glemt password knappen til at virke efter hensigten
</commit_message>
<xml_diff>
--- a/Afsluttende Projekt/Assets/Brugerdata.xlsx
+++ b/Afsluttende Projekt/Assets/Brugerdata.xlsx
@@ -15,7 +15,7 @@
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" fullCalcOnLoad="1" fullPrecision="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,26 +39,27 @@
     <t>Bjarke</t>
   </si>
   <si>
+    <t>Hejmeddig1!</t>
+  </si>
+  <si>
     <t>Andreas</t>
   </si>
   <si>
+    <t>Password2!</t>
+  </si>
+  <si>
     <t>Christoffer</t>
   </si>
   <si>
     <t>Password3!</t>
-  </si>
-  <si>
-    <t>Password2!</t>
-  </si>
-  <si>
-    <t>Password1!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,51 +383,52 @@
     <col min="3" max="3" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2">
+      <c r="A2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="0">
         <v>101</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0">
+        <v>102</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="0">
+        <v>1</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>102</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>